<commit_message>
manage Audit Excel Design Change
</commit_message>
<xml_diff>
--- a/src/assets/files/Manage_Audit.xlsx
+++ b/src/assets/files/Manage_Audit.xlsx
@@ -73,9 +73,9 @@
     <font>
       <b val="true"/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <color rgb="FF211E1E"/>
+      <name val="Consolas"/>
+      <family val="3"/>
       <charset val="1"/>
     </font>
     <font>
@@ -95,17 +95,45 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF4F81BD"/>
-        <bgColor rgb="FF808080"/>
+        <fgColor rgb="FF24989B"/>
+        <bgColor rgb="FF008080"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -134,36 +162,40 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -171,8 +203,12 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -240,16 +276,16 @@
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF4F81BD"/>
+      <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF24989B"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="FF211E1E"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -260,10 +296,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="A:F"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -272,14 +308,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="15.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="15.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="29.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="15.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="31.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
@@ -288,23 +324,44 @@
       <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="8"/>
+      <c r="I1" s="9"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="11"/>
+      <c r="E3" s="10"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="13"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>